<commit_message>
Added results for Ryzen 7 2700X@3.7GHz.
</commit_message>
<xml_diff>
--- a/results/runtime.xlsx
+++ b/results/runtime.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="i7-7700K@4.2GHz" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="i5-6500@3.2GHz" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ryzen 7 2700X@3.7GHz" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t xml:space="preserve">benchmark</t>
   </si>
@@ -242,15 +243,15 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.5"/>
   </cols>
   <sheetData>
@@ -633,17 +634,781 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.66"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>6.98</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>6.96</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>16460</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>6.61</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>124964</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>602276</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>469232</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>7.45</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1336556</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>6.13</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>7.29</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>73764</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>79404</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>3468</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>3416</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>3556</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>3528</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>17652</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>6.14</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>125768</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>603268</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>470460</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>6.96</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>6.68</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1337696</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>75152</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>81740</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added PLATFORM variable to run section.
</commit_message>
<xml_diff>
--- a/results/runtime.xlsx
+++ b/results/runtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konze/Programming/mibench/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D1CCB1-4697-5A44-A136-E5D8083882FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E9BEE-B636-9044-A0AD-0F6BE6CAE2D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="36340" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3019,14 +3019,14 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="42" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>

</xml_diff>